<commit_message>
updated w/ Jeffs new functions
</commit_message>
<xml_diff>
--- a/RemoteSensing/MultispectralBands.xlsx
+++ b/RemoteSensing/MultispectralBands.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dozie\Box Sync\OneDrive\MATLAB\Data\RemSens\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f55e35ae008cf782/MATLAB/JeffFunctionLib/RemoteSensing/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="85" documentId="11_4EEB95108761FF4D7D325296F5D2B40AB17A115C" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C58764E6-CF86-452D-B844-AC584F5FBB0E}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="7365" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11746" firstSheet="7" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VIIRS" sheetId="2" r:id="rId1"/>
@@ -24,6 +25,9 @@
     <sheet name="Sentinel-2" sheetId="11" r:id="rId10"/>
     <sheet name="Himawari-8" sheetId="12" r:id="rId11"/>
     <sheet name="Himawari-9" sheetId="13" r:id="rId12"/>
+    <sheet name="GEO-KOMPSAT-2A" sheetId="16" r:id="rId13"/>
+    <sheet name="Sentinel-3a" sheetId="17" r:id="rId14"/>
+    <sheet name="Sentinel-3b" sheetId="18" r:id="rId15"/>
   </sheets>
   <definedNames>
     <definedName name="atbl" localSheetId="1">ASTER!$A$1:$E$15</definedName>
@@ -32,18 +36,26 @@
     <definedName name="atbl" localSheetId="6">LandsatTM!$A$1:$E$9</definedName>
     <definedName name="atbl" localSheetId="4">MODIS!$A$1:$E$37</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="atbl" type="6" refreshedVersion="6" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="atbl" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\Users\Dozie\Box Sync\OneDrive\MATLAB\Data\RemSens\atbl.txt" comma="1">
       <textFields count="5">
         <textField/>
@@ -54,7 +66,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="atbl1" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="atbl1" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\Users\Dozie\Box Sync\OneDrive\MATLAB\Data\RemSens\atbl.txt" comma="1">
       <textFields count="5">
         <textField/>
@@ -65,7 +77,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="atbl2" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="3" xr16:uid="{00000000-0015-0000-FFFF-FFFF02000000}" name="atbl2" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\Users\Dozie\Box Sync\OneDrive\MATLAB\Data\RemSens\atbl.txt" comma="1">
       <textFields count="5">
         <textField/>
@@ -76,7 +88,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" name="atbl3" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="4" xr16:uid="{00000000-0015-0000-FFFF-FFFF03000000}" name="atbl3" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\Users\Dozie\Box Sync\OneDrive\MATLAB\Data\RemSens\atbl.txt" comma="1">
       <textFields count="5">
         <textField/>
@@ -87,7 +99,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="5" name="atbl4" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="5" xr16:uid="{00000000-0015-0000-FFFF-FFFF04000000}" name="atbl4" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\Users\Dozie\Box Sync\OneDrive\MATLAB\Data\RemSens\atbl.txt" comma="1">
       <textFields count="5">
         <textField/>
@@ -102,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="60">
   <si>
     <t>M1</t>
   </si>
@@ -224,12 +236,6 @@
     <t>LandsatTM</t>
   </si>
   <si>
-    <t>LandsatOLI</t>
-  </si>
-  <si>
-    <t>LandsatTIRS</t>
-  </si>
-  <si>
     <t>B1</t>
   </si>
   <si>
@@ -276,12 +282,24 @@
   </si>
   <si>
     <t>http://www.goes-r.gov/spacesegment/ABI-tech-summary.html</t>
+  </si>
+  <si>
+    <t>Landsat8OLI</t>
+  </si>
+  <si>
+    <t>Landsat8TIRS</t>
+  </si>
+  <si>
+    <t>Sentinel-3a</t>
+  </si>
+  <si>
+    <t>Sentinel-3b</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
@@ -338,7 +356,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -360,6 +378,34 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -381,23 +427,23 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="atbl" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="atbl" connectionId="1" xr16:uid="{00000000-0016-0000-0100-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="atbl" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="atbl" connectionId="2" xr16:uid="{00000000-0016-0000-0200-000001000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="atbl" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="atbl" connectionId="3" xr16:uid="{00000000-0016-0000-0300-000002000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="atbl" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="atbl" connectionId="4" xr16:uid="{00000000-0016-0000-0400-000003000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="atbl" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="atbl" connectionId="5" xr16:uid="{00000000-0016-0000-0600-000004000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -696,7 +742,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1104,7 +1150,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A6:E21">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:E21">
     <sortCondition ref="C6:C21"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1112,11 +1158,11 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+      <selection activeCell="A2" sqref="A2:J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1133,16 +1179,16 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" s="3"/>
-      <c r="B1" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C1" s="9"/>
+      <c r="B1" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="19"/>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
-      <c r="F1" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="G1" s="9"/>
+      <c r="F1" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="19"/>
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
       <c r="J1" s="3"/>
@@ -1150,23 +1196,23 @@
     <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
       <c r="J2" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.45">
@@ -1459,7 +1505,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B11" s="5">
         <v>864.8</v>
@@ -1648,11 +1694,11 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E17"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1683,7 +1729,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1700,7 +1746,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1717,7 +1763,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -1734,7 +1780,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -1751,7 +1797,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -1768,7 +1814,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -1785,7 +1831,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -1802,7 +1848,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -1819,7 +1865,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -1836,7 +1882,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -1853,7 +1899,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -1870,7 +1916,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -1887,7 +1933,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -1904,7 +1950,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -1921,7 +1967,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -1938,7 +1984,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -1960,7 +2006,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1995,7 +2041,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2012,7 +2058,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -2029,7 +2075,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -2046,7 +2092,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -2063,7 +2109,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -2080,7 +2126,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -2097,7 +2143,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -2114,7 +2160,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -2131,7 +2177,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -2148,7 +2194,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -2165,7 +2211,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -2182,7 +2228,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -2199,7 +2245,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -2216,7 +2262,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -2233,7 +2279,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -2250,7 +2296,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -2271,8 +2317,1213 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{541EA15B-059B-48DC-9611-69EC3C15AB7D}">
+  <dimension ref="A2:F18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="16384" width="9.06640625" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="12">
+        <v>1</v>
+      </c>
+      <c r="B3" s="13">
+        <v>470</v>
+      </c>
+      <c r="C3" s="13">
+        <v>41</v>
+      </c>
+      <c r="D3" s="14">
+        <f>(B3-C3/2)/1000</f>
+        <v>0.44950000000000001</v>
+      </c>
+      <c r="E3" s="14">
+        <f t="shared" ref="E3:E16" si="0">(B3+C3/2)/1000</f>
+        <v>0.49049999999999999</v>
+      </c>
+      <c r="F3" s="13">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="12">
+        <v>2</v>
+      </c>
+      <c r="B4" s="13">
+        <v>509</v>
+      </c>
+      <c r="C4" s="13">
+        <v>29</v>
+      </c>
+      <c r="D4" s="14">
+        <f t="shared" ref="D4:D16" si="1">(B4-C4/2)/1000</f>
+        <v>0.4945</v>
+      </c>
+      <c r="E4" s="14">
+        <f t="shared" si="0"/>
+        <v>0.52349999999999997</v>
+      </c>
+      <c r="F4" s="13">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="12">
+        <v>3</v>
+      </c>
+      <c r="B5" s="13">
+        <v>639</v>
+      </c>
+      <c r="C5" s="13">
+        <v>81</v>
+      </c>
+      <c r="D5" s="14">
+        <f t="shared" si="1"/>
+        <v>0.59850000000000003</v>
+      </c>
+      <c r="E5" s="14">
+        <f t="shared" si="0"/>
+        <v>0.67949999999999999</v>
+      </c>
+      <c r="F5" s="13">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="12">
+        <v>4</v>
+      </c>
+      <c r="B6" s="13">
+        <v>863</v>
+      </c>
+      <c r="C6" s="13">
+        <v>34</v>
+      </c>
+      <c r="D6" s="14">
+        <f t="shared" si="1"/>
+        <v>0.84599999999999997</v>
+      </c>
+      <c r="E6" s="14">
+        <f t="shared" si="0"/>
+        <v>0.88</v>
+      </c>
+      <c r="F6" s="13">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="12">
+        <v>5</v>
+      </c>
+      <c r="B7" s="13">
+        <v>1370</v>
+      </c>
+      <c r="C7" s="13">
+        <v>15</v>
+      </c>
+      <c r="D7" s="14">
+        <f t="shared" si="1"/>
+        <v>1.3625</v>
+      </c>
+      <c r="E7" s="14">
+        <f t="shared" si="0"/>
+        <v>1.3774999999999999</v>
+      </c>
+      <c r="F7" s="13">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" s="12">
+        <v>6</v>
+      </c>
+      <c r="B8" s="13">
+        <v>1610</v>
+      </c>
+      <c r="C8" s="13">
+        <v>41</v>
+      </c>
+      <c r="D8" s="14">
+        <f t="shared" si="1"/>
+        <v>1.5894999999999999</v>
+      </c>
+      <c r="E8" s="14">
+        <f t="shared" si="0"/>
+        <v>1.6305000000000001</v>
+      </c>
+      <c r="F8" s="13">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="12">
+        <v>7</v>
+      </c>
+      <c r="B9" s="13">
+        <v>3830</v>
+      </c>
+      <c r="C9" s="13">
+        <f>0.19*1000</f>
+        <v>190</v>
+      </c>
+      <c r="D9" s="14">
+        <f t="shared" si="1"/>
+        <v>3.7349999999999999</v>
+      </c>
+      <c r="E9" s="14">
+        <f t="shared" si="0"/>
+        <v>3.9249999999999998</v>
+      </c>
+      <c r="F9" s="13">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="12">
+        <v>8</v>
+      </c>
+      <c r="B10" s="13">
+        <v>6210</v>
+      </c>
+      <c r="C10" s="13">
+        <f>0.84*1000</f>
+        <v>840</v>
+      </c>
+      <c r="D10" s="14">
+        <f t="shared" si="1"/>
+        <v>5.79</v>
+      </c>
+      <c r="E10" s="14">
+        <f t="shared" si="0"/>
+        <v>6.63</v>
+      </c>
+      <c r="F10" s="13">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" s="12">
+        <v>9</v>
+      </c>
+      <c r="B11" s="13">
+        <v>6940</v>
+      </c>
+      <c r="C11" s="13">
+        <v>400</v>
+      </c>
+      <c r="D11" s="14">
+        <f t="shared" si="1"/>
+        <v>6.74</v>
+      </c>
+      <c r="E11" s="14">
+        <f t="shared" si="0"/>
+        <v>7.14</v>
+      </c>
+      <c r="F11" s="13">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" s="12">
+        <v>10</v>
+      </c>
+      <c r="B12" s="13">
+        <v>7330</v>
+      </c>
+      <c r="C12" s="13">
+        <v>180</v>
+      </c>
+      <c r="D12" s="14">
+        <f t="shared" si="1"/>
+        <v>7.24</v>
+      </c>
+      <c r="E12" s="14">
+        <f t="shared" si="0"/>
+        <v>7.42</v>
+      </c>
+      <c r="F12" s="13">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" s="12">
+        <v>11</v>
+      </c>
+      <c r="B13" s="13">
+        <v>8590</v>
+      </c>
+      <c r="C13" s="13">
+        <v>350</v>
+      </c>
+      <c r="D13" s="14">
+        <f t="shared" si="1"/>
+        <v>8.4149999999999991</v>
+      </c>
+      <c r="E13" s="14">
+        <f t="shared" si="0"/>
+        <v>8.7650000000000006</v>
+      </c>
+      <c r="F13" s="13">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" s="12">
+        <v>12</v>
+      </c>
+      <c r="B14" s="13">
+        <v>9620</v>
+      </c>
+      <c r="C14" s="13">
+        <v>380</v>
+      </c>
+      <c r="D14" s="14">
+        <f t="shared" si="1"/>
+        <v>9.43</v>
+      </c>
+      <c r="E14" s="14">
+        <f t="shared" si="0"/>
+        <v>9.81</v>
+      </c>
+      <c r="F14" s="13">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15" s="15">
+        <v>13</v>
+      </c>
+      <c r="B15" s="16">
+        <v>10350</v>
+      </c>
+      <c r="C15" s="16">
+        <v>470</v>
+      </c>
+      <c r="D15" s="17">
+        <f t="shared" si="1"/>
+        <v>10.115</v>
+      </c>
+      <c r="E15" s="17">
+        <f t="shared" si="0"/>
+        <v>10.585000000000001</v>
+      </c>
+      <c r="F15" s="13">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" s="15">
+        <v>14</v>
+      </c>
+      <c r="B16" s="16">
+        <v>11230</v>
+      </c>
+      <c r="C16" s="16">
+        <v>660</v>
+      </c>
+      <c r="D16" s="17">
+        <f t="shared" si="1"/>
+        <v>10.9</v>
+      </c>
+      <c r="E16" s="17">
+        <f t="shared" si="0"/>
+        <v>11.56</v>
+      </c>
+      <c r="F16" s="13">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17" s="15">
+        <v>15</v>
+      </c>
+      <c r="B17" s="16">
+        <v>12360</v>
+      </c>
+      <c r="C17" s="18">
+        <f>1.11*1000</f>
+        <v>1110</v>
+      </c>
+      <c r="D17" s="17">
+        <f t="shared" ref="D17" si="2">(B17-C17/2)/1000</f>
+        <v>11.805</v>
+      </c>
+      <c r="E17" s="17">
+        <f t="shared" ref="E17" si="3">(B17+C17/2)/1000</f>
+        <v>12.914999999999999</v>
+      </c>
+      <c r="F17" s="13">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18" s="15">
+        <v>16</v>
+      </c>
+      <c r="B18" s="16">
+        <v>13290</v>
+      </c>
+      <c r="C18" s="16">
+        <v>570</v>
+      </c>
+      <c r="D18" s="17">
+        <f t="shared" ref="D18" si="4">(B18-C18/2)/1000</f>
+        <v>13.005000000000001</v>
+      </c>
+      <c r="E18" s="17">
+        <f t="shared" ref="E18" si="5">(B18+C18/2)/1000</f>
+        <v>13.574999999999999</v>
+      </c>
+      <c r="F18" s="13">
+        <v>2000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7725833-3DA8-4E09-AF90-FD957AC2C5AC}">
+  <dimension ref="A1:E22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0.3932967</v>
+      </c>
+      <c r="D2">
+        <v>0.40730959999999999</v>
+      </c>
+      <c r="E2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3">
+        <f>B2+1</f>
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>0.4069238</v>
+      </c>
+      <c r="D3">
+        <v>0.4167669</v>
+      </c>
+      <c r="E3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ref="B4:B22" si="0">B3+1</f>
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>0.43799139999999998</v>
+      </c>
+      <c r="D4">
+        <v>0.44793379999999999</v>
+      </c>
+      <c r="E4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>0.48549720000000002</v>
+      </c>
+      <c r="D5">
+        <v>0.49548880000000001</v>
+      </c>
+      <c r="E5">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>0.50548930000000003</v>
+      </c>
+      <c r="D6">
+        <v>0.51544590000000001</v>
+      </c>
+      <c r="E6">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>0.55544729999999998</v>
+      </c>
+      <c r="D7">
+        <v>0.56545319999999999</v>
+      </c>
+      <c r="E7">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>0.61544019999999999</v>
+      </c>
+      <c r="D8">
+        <v>0.62537830000000005</v>
+      </c>
+      <c r="E8">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>0.66028109999999995</v>
+      </c>
+      <c r="D9">
+        <v>0.67026770000000002</v>
+      </c>
+      <c r="E9">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>0.67026220000000003</v>
+      </c>
+      <c r="D10">
+        <v>0.6777881</v>
+      </c>
+      <c r="E10">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>0.67780660000000004</v>
+      </c>
+      <c r="D11">
+        <v>0.68533429999999995</v>
+      </c>
+      <c r="E11">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>0.70410859999999997</v>
+      </c>
+      <c r="D12">
+        <v>0.71412120000000001</v>
+      </c>
+      <c r="E12">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>0.75042549999999997</v>
+      </c>
+      <c r="D13">
+        <v>0.75793719999999998</v>
+      </c>
+      <c r="E13">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>0.76040819999999998</v>
+      </c>
+      <c r="D14">
+        <v>0.7630441</v>
+      </c>
+      <c r="E14">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>0.76296600000000003</v>
+      </c>
+      <c r="D15">
+        <v>0.76668329999999996</v>
+      </c>
+      <c r="E15">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>0.76661239999999997</v>
+      </c>
+      <c r="D16">
+        <v>0.76922259999999998</v>
+      </c>
+      <c r="E16">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>0.77174960000000004</v>
+      </c>
+      <c r="D17">
+        <v>0.78676380000000001</v>
+      </c>
+      <c r="E17">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>0.8554524</v>
+      </c>
+      <c r="D18">
+        <v>0.87540700000000005</v>
+      </c>
+      <c r="E18">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>0.87931999999999999</v>
+      </c>
+      <c r="D19">
+        <v>0.8892968</v>
+      </c>
+      <c r="E19">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <v>0.89432880000000003</v>
+      </c>
+      <c r="D20">
+        <v>0.90429289999999996</v>
+      </c>
+      <c r="E20">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <v>0.92904439999999999</v>
+      </c>
+      <c r="D21">
+        <v>0.94890180000000002</v>
+      </c>
+      <c r="E21">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="C22">
+        <v>1.0022802</v>
+      </c>
+      <c r="D22">
+        <v>1.0293181</v>
+      </c>
+      <c r="E22">
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90C2DA93-AF36-4389-9F80-5475C541F420}">
+  <dimension ref="A1:E22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0.39392359999999998</v>
+      </c>
+      <c r="D2">
+        <v>0.40726590000000001</v>
+      </c>
+      <c r="E2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3">
+        <f>B2+1</f>
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>0.40701579999999998</v>
+      </c>
+      <c r="D3">
+        <v>0.41688599999999998</v>
+      </c>
+      <c r="E3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ref="B4:B22" si="0">B3+1</f>
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>0.438025</v>
+      </c>
+      <c r="D4">
+        <v>0.4479514</v>
+      </c>
+      <c r="E4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>0.48540810000000001</v>
+      </c>
+      <c r="D5">
+        <v>0.4953901</v>
+      </c>
+      <c r="E5">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>0.50541769999999997</v>
+      </c>
+      <c r="D6">
+        <v>0.51538669999999998</v>
+      </c>
+      <c r="E6">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>0.55536839999999998</v>
+      </c>
+      <c r="D7">
+        <v>0.56536439999999999</v>
+      </c>
+      <c r="E7">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>0.61531910000000001</v>
+      </c>
+      <c r="D8">
+        <v>0.6252489</v>
+      </c>
+      <c r="E8">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>0.66014269999999997</v>
+      </c>
+      <c r="D9">
+        <v>0.67011980000000004</v>
+      </c>
+      <c r="E9">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>0.67011799999999999</v>
+      </c>
+      <c r="D10">
+        <v>0.67761830000000001</v>
+      </c>
+      <c r="E10">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>0.67762540000000004</v>
+      </c>
+      <c r="D11">
+        <v>0.68514569999999997</v>
+      </c>
+      <c r="E11">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>0.70397750000000003</v>
+      </c>
+      <c r="D12">
+        <v>0.71398660000000003</v>
+      </c>
+      <c r="E12">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>0.75027160000000004</v>
+      </c>
+      <c r="D13">
+        <v>0.75778509999999999</v>
+      </c>
+      <c r="E13">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>0.76025940000000003</v>
+      </c>
+      <c r="D14">
+        <v>0.76285950000000002</v>
+      </c>
+      <c r="E14">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>0.76281310000000002</v>
+      </c>
+      <c r="D15">
+        <v>0.76657140000000001</v>
+      </c>
+      <c r="E15">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>0.7665265</v>
+      </c>
+      <c r="D16">
+        <v>0.76911839999999998</v>
+      </c>
+      <c r="E16">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>0.77157770000000003</v>
+      </c>
+      <c r="D17">
+        <v>0.78658039999999996</v>
+      </c>
+      <c r="E17">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>0.85530479999999998</v>
+      </c>
+      <c r="D18">
+        <v>0.8752373</v>
+      </c>
+      <c r="E18">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>0.87914499999999995</v>
+      </c>
+      <c r="D19">
+        <v>0.8891097</v>
+      </c>
+      <c r="E19">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <v>0.89414179999999999</v>
+      </c>
+      <c r="D20">
+        <v>0.90410140000000006</v>
+      </c>
+      <c r="E20">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <v>0.92887549999999997</v>
+      </c>
+      <c r="D21">
+        <v>0.9487196</v>
+      </c>
+      <c r="E21">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="C22">
+        <v>1.0022788</v>
+      </c>
+      <c r="D22">
+        <v>1.0291888</v>
+      </c>
+      <c r="E22">
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2550,7 +3801,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2691,7 +3942,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2815,7 +4066,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2848,7 +4099,7 @@
         <v>27</v>
       </c>
       <c r="F1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
@@ -3577,10 +4828,10 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:D18"/>
     </sheetView>
   </sheetViews>
@@ -3593,13 +4844,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A1" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
+      <c r="A1" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
@@ -3849,7 +5100,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4024,11 +5275,11 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4059,7 +5310,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -4076,7 +5327,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
@@ -4093,7 +5344,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="B4" s="1">
         <v>3</v>
@@ -4110,7 +5361,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="B5" s="1">
         <v>4</v>
@@ -4127,7 +5378,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="B6" s="1">
         <v>5</v>
@@ -4144,7 +5395,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="B7" s="1">
         <v>6</v>
@@ -4161,7 +5412,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="B8" s="1">
         <v>7</v>
@@ -4178,7 +5429,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="B9" s="1">
         <v>8</v>
@@ -4195,7 +5446,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="B10" s="1">
         <v>9</v>
@@ -4212,7 +5463,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="B11" s="1">
         <v>10</v>
@@ -4229,7 +5480,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="B12" s="1">
         <v>11</v>
@@ -4250,7 +5501,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4285,10 +5536,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C2">
         <v>0.5</v>
@@ -4302,10 +5553,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C3">
         <v>0.61</v>
@@ -4319,10 +5570,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C4">
         <v>0.79</v>
@@ -4336,10 +5587,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C5">
         <v>1.58</v>
@@ -4353,10 +5604,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C6">
         <v>0.5</v>

</xml_diff>